<commit_message>
create  a mfc project
</commit_message>
<xml_diff>
--- a/scada工程进度安排表.xlsx
+++ b/scada工程进度安排表.xlsx
@@ -523,40 +523,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -923,22 +923,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="39.375" customWidth="1"/>
+    <col min="3" max="3" width="41.75" customWidth="1"/>
     <col min="4" max="4" width="22.75" customWidth="1"/>
     <col min="5" max="5" width="13.375" customWidth="1"/>
     <col min="6" max="6" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="58.5" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" s="17" customFormat="1" ht="58.5" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1006,53 +1006,53 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="22.5">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="15" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1068,19 +1068,19 @@
     </row>
     <row r="19" spans="1:11" ht="22.5" customHeight="1">
       <c r="A19" s="5"/>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="5"/>
@@ -1090,94 +1090,94 @@
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="18.75">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:11" ht="18.75">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:11" ht="18.75">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:11" ht="18.75">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:11" ht="18.75">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:11" ht="18.75">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="8"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:11">
       <c r="B26" s="4"/>
@@ -1218,11 +1218,11 @@
       <c r="A31" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
@@ -1230,47 +1230,47 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="22.5">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
@@ -1278,73 +1278,73 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="22.5">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="16"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" s="17" t="s">
+      <c r="D40" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F40" s="16"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" s="17" t="s">
+      <c r="D41" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F41" s="16"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>